<commit_message>
feat(06-02): generate all 5 scenario sheets with correct preset values
- Scenario A - 3K: Revenue 3000, Expenses 750, Belgium 1000
- Scenario B - 6K: Revenue 6000, Expenses 1500, Belgium 1000
- Scenario C - 9K: Revenue 9000, Expenses 3000, Belgium 2500
- Scenario D - 12K: Revenue 12000, Expenses 5000, Belgium 2500
- Scenario E - 18K: Revenue 18000, Expenses 8000, Belgium 2500
- Belgium patterns match CLAUDE.md: A/B low (1000), C/D/E high (2500)
- All formulas use named ranges and recalculate when inputs change

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/autonomo_calculator.xlsx
+++ b/autonomo_calculator.xlsx
@@ -5,6 +5,11 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Constants" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Scenario A - 3K" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Scenario B - 6K" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Scenario C - 9K" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Scenario D - 12K" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="Scenario E - 18K" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="RETA_MONTHLY">Constants!$B$5</definedName>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="57">
   <si>
     <t>Fiscal Data 2025/2026</t>
   </si>
@@ -89,6 +94,108 @@
   </si>
   <si>
     <t>- Update these values for 2027 rates when available</t>
+  </si>
+  <si>
+    <t>INPUTS (Edit these values)</t>
+  </si>
+  <si>
+    <t>Monthly Revenue</t>
+  </si>
+  <si>
+    <t>Monthly Expenses</t>
+  </si>
+  <si>
+    <t>Belgium Pattern</t>
+  </si>
+  <si>
+    <t>Spain Deductible</t>
+  </si>
+  <si>
+    <t>ANNUAL CALCULATIONS</t>
+  </si>
+  <si>
+    <t>Annual Revenue</t>
+  </si>
+  <si>
+    <t>Annual Expenses</t>
+  </si>
+  <si>
+    <t>Annual Belgium Costs</t>
+  </si>
+  <si>
+    <t>Annual Spain Deductible</t>
+  </si>
+  <si>
+    <t>Total Deductible</t>
+  </si>
+  <si>
+    <t>Rendimiento Neto Previo</t>
+  </si>
+  <si>
+    <t>GASTOS DE DIFICIL JUSTIFICACION</t>
+  </si>
+  <si>
+    <t>Gastos Dificil (5%)</t>
+  </si>
+  <si>
+    <t>Base Liquidable</t>
+  </si>
+  <si>
+    <t>IRPF BRACKET CALCULATION</t>
+  </si>
+  <si>
+    <t>Taxable</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Total Tax (Cuota 1)</t>
+  </si>
+  <si>
+    <t>4-PHASE MINIMO METHOD</t>
+  </si>
+  <si>
+    <t>Tax on Base (Cuota 1)</t>
+  </si>
+  <si>
+    <t>Minimo Descendientes</t>
+  </si>
+  <si>
+    <t>Total Minimos</t>
+  </si>
+  <si>
+    <t>Tax on Minimos (Cuota 3)</t>
+  </si>
+  <si>
+    <t>Cuota Integra</t>
+  </si>
+  <si>
+    <t>Cuota Diferencial</t>
+  </si>
+  <si>
+    <t>FINAL RESULTS</t>
+  </si>
+  <si>
+    <t>Annual IRPF</t>
+  </si>
+  <si>
+    <t>Monthly IRPF</t>
+  </si>
+  <si>
+    <t>Annual Net Income</t>
+  </si>
+  <si>
+    <t>Monthly Net Income</t>
+  </si>
+  <si>
+    <t>Annual Leefgeld</t>
+  </si>
+  <si>
+    <t>Monthly Leefgeld</t>
+  </si>
+  <si>
+    <t>Effective Tax Rate</t>
   </si>
 </sst>
 </file>
@@ -120,7 +227,7 @@
       <b/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +237,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE0E0E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0F0FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -145,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -155,11 +267,330 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -722,4 +1153,2349 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E53"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="9">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4">
+        <f>B3*12</f>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <f>B4*12</f>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B5*12</f>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4">
+        <f>B6*12</f>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4">
+        <f>RETA_ANNUAL</f>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="10">
+        <f>SUM(B11:B14)</f>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="10">
+        <f>B10-B15</f>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B16</f>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4">
+        <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="10">
+        <f>MAX(0,B16-B21)</f>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5">
+        <v>12450</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="D26" s="4">
+        <f>MAX(0,MIN($B$22,12450)-0)</f>
+      </c>
+      <c r="E26" s="4">
+        <f>D26*C26</f>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>12450</v>
+      </c>
+      <c r="B27" s="5">
+        <v>20200</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D27" s="4">
+        <f>MAX(0,MIN($B$22,20200)-12450)</f>
+      </c>
+      <c r="E27" s="4">
+        <f>D27*C27</f>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>20200</v>
+      </c>
+      <c r="B28" s="5">
+        <v>35200</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="D28" s="4">
+        <f>MAX(0,MIN($B$22,35200)-20200)</f>
+      </c>
+      <c r="E28" s="4">
+        <f>D28*C28</f>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>35200</v>
+      </c>
+      <c r="B29" s="5">
+        <v>60000</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="D29" s="4">
+        <f>MAX(0,MIN($B$22,60000)-35200)</f>
+      </c>
+      <c r="E29" s="4">
+        <f>D29*C29</f>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>60000</v>
+      </c>
+      <c r="B30" s="5">
+        <v>300000</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="D30" s="4">
+        <f>MAX(0,MIN($B$22,300000)-60000)</f>
+      </c>
+      <c r="E30" s="4">
+        <f>D30*C30</f>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>300000</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="D31" s="4">
+        <f>MAX(0,MIN($B$22,999999999)-300000)</f>
+      </c>
+      <c r="E31" s="4">
+        <f>D31*C31</f>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="10">
+        <f>SUM(E26:E31)</f>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4">
+        <f>B22</f>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="4">
+        <f>E32</f>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="5">
+        <f>MINIMO_PERSONAL</f>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="5">
+        <f>MINIMO_DESCENDIENTES</f>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="11">
+        <f>B38+B39</f>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="4">
+        <f>B40*0.19</f>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="10">
+        <f>MAX(0,B37-B41)</f>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="10">
+        <f>B42</f>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4">
+        <f>B43</f>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="4">
+        <f>B47/12</f>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="10">
+        <f>B10-B15-B47</f>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="10">
+        <f>B49/12</f>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="10">
+        <f>B49-(PRIVATE_COSTS*12)</f>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="10">
+        <f>B51/12</f>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="6">
+        <f>IFERROR(B47/B16,0)</f>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A45:C45"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B51">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
+      <formula>0.3</formula>
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
+      <formula>0.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="B5">
+      <formula1>"1000,2500"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E53"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="9">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4">
+        <f>B3*12</f>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <f>B4*12</f>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B5*12</f>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4">
+        <f>B6*12</f>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4">
+        <f>RETA_ANNUAL</f>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="10">
+        <f>SUM(B11:B14)</f>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="10">
+        <f>B10-B15</f>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B16</f>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4">
+        <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="10">
+        <f>MAX(0,B16-B21)</f>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5">
+        <v>12450</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="D26" s="4">
+        <f>MAX(0,MIN($B$22,12450)-0)</f>
+      </c>
+      <c r="E26" s="4">
+        <f>D26*C26</f>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>12450</v>
+      </c>
+      <c r="B27" s="5">
+        <v>20200</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D27" s="4">
+        <f>MAX(0,MIN($B$22,20200)-12450)</f>
+      </c>
+      <c r="E27" s="4">
+        <f>D27*C27</f>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>20200</v>
+      </c>
+      <c r="B28" s="5">
+        <v>35200</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="D28" s="4">
+        <f>MAX(0,MIN($B$22,35200)-20200)</f>
+      </c>
+      <c r="E28" s="4">
+        <f>D28*C28</f>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>35200</v>
+      </c>
+      <c r="B29" s="5">
+        <v>60000</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="D29" s="4">
+        <f>MAX(0,MIN($B$22,60000)-35200)</f>
+      </c>
+      <c r="E29" s="4">
+        <f>D29*C29</f>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>60000</v>
+      </c>
+      <c r="B30" s="5">
+        <v>300000</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="D30" s="4">
+        <f>MAX(0,MIN($B$22,300000)-60000)</f>
+      </c>
+      <c r="E30" s="4">
+        <f>D30*C30</f>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>300000</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="D31" s="4">
+        <f>MAX(0,MIN($B$22,999999999)-300000)</f>
+      </c>
+      <c r="E31" s="4">
+        <f>D31*C31</f>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="10">
+        <f>SUM(E26:E31)</f>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4">
+        <f>B22</f>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="4">
+        <f>E32</f>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="5">
+        <f>MINIMO_PERSONAL</f>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="5">
+        <f>MINIMO_DESCENDIENTES</f>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="11">
+        <f>B38+B39</f>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="4">
+        <f>B40*0.19</f>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="10">
+        <f>MAX(0,B37-B41)</f>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="10">
+        <f>B42</f>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4">
+        <f>B43</f>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="4">
+        <f>B47/12</f>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="10">
+        <f>B10-B15-B47</f>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="10">
+        <f>B49/12</f>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="10">
+        <f>B49-(PRIVATE_COSTS*12)</f>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="10">
+        <f>B51/12</f>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="6">
+        <f>IFERROR(B47/B16,0)</f>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A45:C45"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B51">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="greaterThan">
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="between">
+      <formula>0.3</formula>
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="lessThan">
+      <formula>0.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="B5">
+      <formula1>"1000,2500"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E53"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="9">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4">
+        <f>B3*12</f>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <f>B4*12</f>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B5*12</f>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4">
+        <f>B6*12</f>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4">
+        <f>RETA_ANNUAL</f>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="10">
+        <f>SUM(B11:B14)</f>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="10">
+        <f>B10-B15</f>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B16</f>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4">
+        <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="10">
+        <f>MAX(0,B16-B21)</f>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5">
+        <v>12450</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="D26" s="4">
+        <f>MAX(0,MIN($B$22,12450)-0)</f>
+      </c>
+      <c r="E26" s="4">
+        <f>D26*C26</f>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>12450</v>
+      </c>
+      <c r="B27" s="5">
+        <v>20200</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D27" s="4">
+        <f>MAX(0,MIN($B$22,20200)-12450)</f>
+      </c>
+      <c r="E27" s="4">
+        <f>D27*C27</f>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>20200</v>
+      </c>
+      <c r="B28" s="5">
+        <v>35200</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="D28" s="4">
+        <f>MAX(0,MIN($B$22,35200)-20200)</f>
+      </c>
+      <c r="E28" s="4">
+        <f>D28*C28</f>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>35200</v>
+      </c>
+      <c r="B29" s="5">
+        <v>60000</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="D29" s="4">
+        <f>MAX(0,MIN($B$22,60000)-35200)</f>
+      </c>
+      <c r="E29" s="4">
+        <f>D29*C29</f>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>60000</v>
+      </c>
+      <c r="B30" s="5">
+        <v>300000</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="D30" s="4">
+        <f>MAX(0,MIN($B$22,300000)-60000)</f>
+      </c>
+      <c r="E30" s="4">
+        <f>D30*C30</f>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>300000</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="D31" s="4">
+        <f>MAX(0,MIN($B$22,999999999)-300000)</f>
+      </c>
+      <c r="E31" s="4">
+        <f>D31*C31</f>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="10">
+        <f>SUM(E26:E31)</f>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4">
+        <f>B22</f>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="4">
+        <f>E32</f>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="5">
+        <f>MINIMO_PERSONAL</f>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="5">
+        <f>MINIMO_DESCENDIENTES</f>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="11">
+        <f>B38+B39</f>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="4">
+        <f>B40*0.19</f>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="10">
+        <f>MAX(0,B37-B41)</f>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="10">
+        <f>B42</f>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4">
+        <f>B43</f>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="4">
+        <f>B47/12</f>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="10">
+        <f>B10-B15-B47</f>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="10">
+        <f>B49/12</f>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="10">
+        <f>B49-(PRIVATE_COSTS*12)</f>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="10">
+        <f>B51/12</f>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="6">
+        <f>IFERROR(B47/B16,0)</f>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A45:C45"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B51">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="greaterThan">
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="between">
+      <formula>0.3</formula>
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="lessThan">
+      <formula>0.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="B5">
+      <formula1>"1000,2500"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E53"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="9">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4">
+        <f>B3*12</f>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <f>B4*12</f>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B5*12</f>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4">
+        <f>B6*12</f>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4">
+        <f>RETA_ANNUAL</f>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="10">
+        <f>SUM(B11:B14)</f>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="10">
+        <f>B10-B15</f>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B16</f>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4">
+        <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="10">
+        <f>MAX(0,B16-B21)</f>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5">
+        <v>12450</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="D26" s="4">
+        <f>MAX(0,MIN($B$22,12450)-0)</f>
+      </c>
+      <c r="E26" s="4">
+        <f>D26*C26</f>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>12450</v>
+      </c>
+      <c r="B27" s="5">
+        <v>20200</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D27" s="4">
+        <f>MAX(0,MIN($B$22,20200)-12450)</f>
+      </c>
+      <c r="E27" s="4">
+        <f>D27*C27</f>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>20200</v>
+      </c>
+      <c r="B28" s="5">
+        <v>35200</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="D28" s="4">
+        <f>MAX(0,MIN($B$22,35200)-20200)</f>
+      </c>
+      <c r="E28" s="4">
+        <f>D28*C28</f>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>35200</v>
+      </c>
+      <c r="B29" s="5">
+        <v>60000</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="D29" s="4">
+        <f>MAX(0,MIN($B$22,60000)-35200)</f>
+      </c>
+      <c r="E29" s="4">
+        <f>D29*C29</f>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>60000</v>
+      </c>
+      <c r="B30" s="5">
+        <v>300000</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="D30" s="4">
+        <f>MAX(0,MIN($B$22,300000)-60000)</f>
+      </c>
+      <c r="E30" s="4">
+        <f>D30*C30</f>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>300000</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="D31" s="4">
+        <f>MAX(0,MIN($B$22,999999999)-300000)</f>
+      </c>
+      <c r="E31" s="4">
+        <f>D31*C31</f>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="10">
+        <f>SUM(E26:E31)</f>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4">
+        <f>B22</f>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="4">
+        <f>E32</f>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="5">
+        <f>MINIMO_PERSONAL</f>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="5">
+        <f>MINIMO_DESCENDIENTES</f>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="11">
+        <f>B38+B39</f>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="4">
+        <f>B40*0.19</f>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="10">
+        <f>MAX(0,B37-B41)</f>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="10">
+        <f>B42</f>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4">
+        <f>B43</f>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="4">
+        <f>B47/12</f>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="10">
+        <f>B10-B15-B47</f>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="10">
+        <f>B49/12</f>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="10">
+        <f>B49-(PRIVATE_COSTS*12)</f>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="10">
+        <f>B51/12</f>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="6">
+        <f>IFERROR(B47/B16,0)</f>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A45:C45"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B51">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="between">
+      <formula>0.3</formula>
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="9" operator="lessThan">
+      <formula>0.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="B5">
+      <formula1>"1000,2500"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E53"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="9">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4">
+        <f>B3*12</f>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <f>B4*12</f>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B5*12</f>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4">
+        <f>B6*12</f>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4">
+        <f>RETA_ANNUAL</f>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="10">
+        <f>SUM(B11:B14)</f>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="10">
+        <f>B10-B15</f>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B16</f>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4">
+        <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="10">
+        <f>MAX(0,B16-B21)</f>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5">
+        <v>12450</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="D26" s="4">
+        <f>MAX(0,MIN($B$22,12450)-0)</f>
+      </c>
+      <c r="E26" s="4">
+        <f>D26*C26</f>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>12450</v>
+      </c>
+      <c r="B27" s="5">
+        <v>20200</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D27" s="4">
+        <f>MAX(0,MIN($B$22,20200)-12450)</f>
+      </c>
+      <c r="E27" s="4">
+        <f>D27*C27</f>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>20200</v>
+      </c>
+      <c r="B28" s="5">
+        <v>35200</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="D28" s="4">
+        <f>MAX(0,MIN($B$22,35200)-20200)</f>
+      </c>
+      <c r="E28" s="4">
+        <f>D28*C28</f>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>35200</v>
+      </c>
+      <c r="B29" s="5">
+        <v>60000</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="D29" s="4">
+        <f>MAX(0,MIN($B$22,60000)-35200)</f>
+      </c>
+      <c r="E29" s="4">
+        <f>D29*C29</f>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>60000</v>
+      </c>
+      <c r="B30" s="5">
+        <v>300000</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="D30" s="4">
+        <f>MAX(0,MIN($B$22,300000)-60000)</f>
+      </c>
+      <c r="E30" s="4">
+        <f>D30*C30</f>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>300000</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="D31" s="4">
+        <f>MAX(0,MIN($B$22,999999999)-300000)</f>
+      </c>
+      <c r="E31" s="4">
+        <f>D31*C31</f>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="10">
+        <f>SUM(E26:E31)</f>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4">
+        <f>B22</f>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="4">
+        <f>E32</f>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="5">
+        <f>MINIMO_PERSONAL</f>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="5">
+        <f>MINIMO_DESCENDIENTES</f>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="11">
+        <f>B38+B39</f>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="4">
+        <f>B40*0.19</f>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="10">
+        <f>MAX(0,B37-B41)</f>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="10">
+        <f>B42</f>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4">
+        <f>B43</f>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="4">
+        <f>B47/12</f>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="10">
+        <f>B10-B15-B47</f>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="10">
+        <f>B49/12</f>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="10">
+        <f>B49-(PRIVATE_COSTS*12)</f>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="10">
+        <f>B51/12</f>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="6">
+        <f>IFERROR(B47/B16,0)</f>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A45:C45"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B51">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="greaterThan">
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="between">
+      <formula>0.3</formula>
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="9" operator="lessThan">
+      <formula>0.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="B5">
+      <formula1>"1000,2500"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(06-03): add Overview sheet with comparison table and navigation
- createOverviewSheet function with navigation hyperlinks to all scenario sheets
- Cross-sheet formulas referencing B3, B5, B10, B15, B22, B47-B53 from each scenario
- Comparison table showing all 5 scenarios side-by-side (A-E columns)
- Conditional formatting on leefgeld rows (red/orange/green thresholds)
- Freeze panes at row 13 (header) and column A (metrics)
- Sheet order: Overview, Scenario A-E, Constants (via orderNo)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/autonomo_calculator.xlsx
+++ b/autonomo_calculator.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Constants" state="visible" r:id="rId4"/>
+    <sheet sheetId="7" name="Overview" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="Scenario A - 3K" state="visible" r:id="rId5"/>
     <sheet sheetId="3" name="Scenario B - 6K" state="visible" r:id="rId6"/>
     <sheet sheetId="4" name="Scenario C - 9K" state="visible" r:id="rId7"/>
     <sheet sheetId="5" name="Scenario D - 12K" state="visible" r:id="rId8"/>
     <sheet sheetId="6" name="Scenario E - 18K" state="visible" r:id="rId9"/>
+    <sheet sheetId="1" name="Constants" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="RETA_MONTHLY">Constants!$B$5</definedName>
@@ -25,7 +26,178 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="74">
+  <si>
+    <t>Spanish Autonomo Tax Calculator</t>
+  </si>
+  <si>
+    <t>Fiscal Year 2025/2026</t>
+  </si>
+  <si>
+    <t>Quick Navigation</t>
+  </si>
+  <si>
+    <t>Scenario A - 3K</t>
+  </si>
+  <si>
+    <t>Scenario B - 6K</t>
+  </si>
+  <si>
+    <t>Scenario C - 9K</t>
+  </si>
+  <si>
+    <t>Scenario D - 12K</t>
+  </si>
+  <si>
+    <t>Scenario E - 18K</t>
+  </si>
+  <si>
+    <t>Constants (Fiscal Data)</t>
+  </si>
+  <si>
+    <t>Scenario Comparison</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Monthly Revenue</t>
+  </si>
+  <si>
+    <t>Monthly Expenses</t>
+  </si>
+  <si>
+    <t>Belgium Pattern</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Annual Revenue</t>
+  </si>
+  <si>
+    <t>Total Deductible</t>
+  </si>
+  <si>
+    <t>Base Liquidable</t>
+  </si>
+  <si>
+    <t>Annual IRPF</t>
+  </si>
+  <si>
+    <t>Monthly IRPF</t>
+  </si>
+  <si>
+    <t>Effective Tax Rate</t>
+  </si>
+  <si>
+    <t>Annual Net Income</t>
+  </si>
+  <si>
+    <t>Monthly Net Income</t>
+  </si>
+  <si>
+    <t>Annual Leefgeld</t>
+  </si>
+  <si>
+    <t>Monthly Leefgeld</t>
+  </si>
+  <si>
+    <t>INPUTS (Edit these values)</t>
+  </si>
+  <si>
+    <t>Spain Deductible</t>
+  </si>
+  <si>
+    <t>ANNUAL CALCULATIONS</t>
+  </si>
+  <si>
+    <t>Annual Expenses</t>
+  </si>
+  <si>
+    <t>Annual Belgium Costs</t>
+  </si>
+  <si>
+    <t>Annual Spain Deductible</t>
+  </si>
+  <si>
+    <t>RETA Annual</t>
+  </si>
+  <si>
+    <t>Rendimiento Neto Previo</t>
+  </si>
+  <si>
+    <t>GASTOS DE DIFICIL JUSTIFICACION</t>
+  </si>
+  <si>
+    <t>Gastos Dificil (5%)</t>
+  </si>
+  <si>
+    <t>IRPF BRACKET CALCULATION</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Taxable</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Total Tax (Cuota 1)</t>
+  </si>
+  <si>
+    <t>4-PHASE MINIMO METHOD</t>
+  </si>
+  <si>
+    <t>Tax on Base (Cuota 1)</t>
+  </si>
+  <si>
+    <t>Minimo Personal</t>
+  </si>
+  <si>
+    <t>Minimo Descendientes</t>
+  </si>
+  <si>
+    <t>Total Minimos</t>
+  </si>
+  <si>
+    <t>Tax on Minimos (Cuota 3)</t>
+  </si>
+  <si>
+    <t>Cuota Integra</t>
+  </si>
+  <si>
+    <t>Cuota Diferencial</t>
+  </si>
+  <si>
+    <t>FINAL RESULTS</t>
+  </si>
   <si>
     <t>Fiscal Data 2025/2026</t>
   </si>
@@ -39,15 +211,9 @@
     <t>RETA Monthly</t>
   </si>
   <si>
-    <t>RETA Annual</t>
-  </si>
-  <si>
     <t>Minimos Personales y Familiares</t>
   </si>
   <si>
-    <t>Minimo Personal</t>
-  </si>
-  <si>
     <t>Minimo Descendientes (1)</t>
   </si>
   <si>
@@ -69,21 +235,9 @@
     <t>IRPF 2025 Brackets</t>
   </si>
   <si>
-    <t>Lower</t>
-  </si>
-  <si>
-    <t>Upper</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
     <t>Base Tax</t>
   </si>
   <si>
-    <t>+</t>
-  </si>
-  <si>
     <t>Notes:</t>
   </si>
   <si>
@@ -94,108 +248,6 @@
   </si>
   <si>
     <t>- Update these values for 2027 rates when available</t>
-  </si>
-  <si>
-    <t>INPUTS (Edit these values)</t>
-  </si>
-  <si>
-    <t>Monthly Revenue</t>
-  </si>
-  <si>
-    <t>Monthly Expenses</t>
-  </si>
-  <si>
-    <t>Belgium Pattern</t>
-  </si>
-  <si>
-    <t>Spain Deductible</t>
-  </si>
-  <si>
-    <t>ANNUAL CALCULATIONS</t>
-  </si>
-  <si>
-    <t>Annual Revenue</t>
-  </si>
-  <si>
-    <t>Annual Expenses</t>
-  </si>
-  <si>
-    <t>Annual Belgium Costs</t>
-  </si>
-  <si>
-    <t>Annual Spain Deductible</t>
-  </si>
-  <si>
-    <t>Total Deductible</t>
-  </si>
-  <si>
-    <t>Rendimiento Neto Previo</t>
-  </si>
-  <si>
-    <t>GASTOS DE DIFICIL JUSTIFICACION</t>
-  </si>
-  <si>
-    <t>Gastos Dificil (5%)</t>
-  </si>
-  <si>
-    <t>Base Liquidable</t>
-  </si>
-  <si>
-    <t>IRPF BRACKET CALCULATION</t>
-  </si>
-  <si>
-    <t>Taxable</t>
-  </si>
-  <si>
-    <t>Tax</t>
-  </si>
-  <si>
-    <t>Total Tax (Cuota 1)</t>
-  </si>
-  <si>
-    <t>4-PHASE MINIMO METHOD</t>
-  </si>
-  <si>
-    <t>Tax on Base (Cuota 1)</t>
-  </si>
-  <si>
-    <t>Minimo Descendientes</t>
-  </si>
-  <si>
-    <t>Total Minimos</t>
-  </si>
-  <si>
-    <t>Tax on Minimos (Cuota 3)</t>
-  </si>
-  <si>
-    <t>Cuota Integra</t>
-  </si>
-  <si>
-    <t>Cuota Diferencial</t>
-  </si>
-  <si>
-    <t>FINAL RESULTS</t>
-  </si>
-  <si>
-    <t>Annual IRPF</t>
-  </si>
-  <si>
-    <t>Monthly IRPF</t>
-  </si>
-  <si>
-    <t>Annual Net Income</t>
-  </si>
-  <si>
-    <t>Monthly Net Income</t>
-  </si>
-  <si>
-    <t>Annual Leefgeld</t>
-  </si>
-  <si>
-    <t>Monthly Leefgeld</t>
-  </si>
-  <si>
-    <t>Effective Tax Rate</t>
   </si>
 </sst>
 </file>
@@ -207,7 +259,7 @@
     <numFmt numFmtId="165" formatCode="&quot;EUR &quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -217,17 +269,29 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+    </font>
+    <font>
+      <color rgb="FF666666"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0066CC"/>
+    </font>
+    <font>
+      <b/>
     </font>
     <font>
       <i/>
       <color rgb="FF666666"/>
     </font>
-    <font>
-      <b/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,12 +300,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE0E0E0"/>
+        <fgColor rgb="FFD0D0D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE0F0FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0E0E0"/>
       </patternFill>
     </fill>
   </fills>
@@ -257,24 +331,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="51">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF6B6B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF4ECDC4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -935,215 +1078,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
+      <c r="A4" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
+        <v>60</v>
+      </c>
+      <c r="B5" s="14">
         <v>428.4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
+        <v>36</v>
+      </c>
+      <c r="B6" s="14">
         <f>RETA_MONTHLY*12</f>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
+      <c r="A8" s="19" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5">
+        <v>50</v>
+      </c>
+      <c r="B9" s="17">
         <v>5550</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5">
+        <v>62</v>
+      </c>
+      <c r="B10" s="17">
         <v>2400</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>8</v>
+      <c r="A12" s="19" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="6">
+        <v>64</v>
+      </c>
+      <c r="B13" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="5">
+        <v>65</v>
+      </c>
+      <c r="B14" s="17">
         <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>11</v>
+      <c r="A16" s="19" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="5">
+        <v>67</v>
+      </c>
+      <c r="B17" s="17">
         <v>1727</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
+      <c r="A19" s="19" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>17</v>
+      <c r="A20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="17">
         <v>0</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="17">
         <v>12450</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="18">
         <v>0.19</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="17">
         <v>12450</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="17">
         <v>20200</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="18">
         <v>0.24</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="14">
         <v>2365.5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="17">
         <v>20200</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="17">
         <v>35200</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="18">
         <v>0.3</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="14">
         <v>4225.5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="17">
         <v>35200</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="17">
         <v>60000</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="18">
         <v>0.37</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="14">
         <v>8725.5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="17">
         <v>60000</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="17">
         <v>300000</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="18">
         <v>0.45</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="14">
         <v>17901.5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="17">
         <v>300000</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="8">
+        <v>46</v>
+      </c>
+      <c r="C26" s="18">
         <v>0.47</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="14">
         <v>125901.5</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>19</v>
+      <c r="A28" s="19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>20</v>
+      <c r="A29" s="22" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>21</v>
+      <c r="A30" s="22" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>22</v>
+      <c r="A31" s="22" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1167,405 +1310,405 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="9">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13">
         <v>3000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="9">
+        <v>17</v>
+      </c>
+      <c r="B4" s="13">
         <v>750</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="9">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9">
+        <v>31</v>
+      </c>
+      <c r="B6" s="13">
         <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14">
         <f>B3*12</f>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4">
+        <v>33</v>
+      </c>
+      <c r="B11" s="14">
         <f>B4*12</f>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="4">
+        <v>34</v>
+      </c>
+      <c r="B12" s="14">
         <f>B5*12</f>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4">
+        <v>35</v>
+      </c>
+      <c r="B13" s="14">
         <f>B6*12</f>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4">
+        <v>36</v>
+      </c>
+      <c r="B14" s="14">
         <f>RETA_ANNUAL</f>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="10">
+        <v>21</v>
+      </c>
+      <c r="B15" s="15">
         <f>SUM(B11:B14)</f>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="10">
+        <v>37</v>
+      </c>
+      <c r="B16" s="15">
         <f>B10-B15</f>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="4">
+        <v>37</v>
+      </c>
+      <c r="B20" s="14">
         <f>B16</f>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="4">
+        <v>39</v>
+      </c>
+      <c r="B21" s="14">
         <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15">
         <f>MAX(0,B16-B21)</f>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>40</v>
+      <c r="A25" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="17">
         <v>0</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="17">
         <v>12450</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="18">
         <v>0.19</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="14">
         <f>MAX(0,MIN($B$22,12450)-0)</f>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="14">
         <f>D26*C26</f>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="17">
         <v>12450</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="17">
         <v>20200</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="18">
         <v>0.24</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="14">
         <f>MAX(0,MIN($B$22,20200)-12450)</f>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="14">
         <f>D27*C27</f>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="17">
         <v>20200</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="17">
         <v>35200</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="18">
         <v>0.3</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="14">
         <f>MAX(0,MIN($B$22,35200)-20200)</f>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="14">
         <f>D28*C28</f>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="17">
         <v>35200</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="17">
         <v>60000</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="18">
         <v>0.37</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="14">
         <f>MAX(0,MIN($B$22,60000)-35200)</f>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="14">
         <f>D29*C29</f>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="17">
         <v>60000</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="17">
         <v>300000</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="18">
         <v>0.45</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="14">
         <f>MAX(0,MIN($B$22,300000)-60000)</f>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="14">
         <f>D30*C30</f>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="17">
         <v>300000</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="8">
+        <v>46</v>
+      </c>
+      <c r="C31" s="18">
         <v>0.47</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="14">
         <f>MAX(0,MIN($B$22,999999999)-300000)</f>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="14">
         <f>D31*C31</f>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="10">
+      <c r="A32" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="15">
         <f>SUM(E26:E31)</f>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="4">
+        <v>22</v>
+      </c>
+      <c r="B36" s="14">
         <f>B22</f>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="4">
+        <v>49</v>
+      </c>
+      <c r="B37" s="14">
         <f>E32</f>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="5">
+        <v>50</v>
+      </c>
+      <c r="B38" s="17">
         <f>MINIMO_PERSONAL</f>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="5">
+        <v>51</v>
+      </c>
+      <c r="B39" s="17">
         <f>MINIMO_DESCENDIENTES</f>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="11">
+        <v>52</v>
+      </c>
+      <c r="B40" s="20">
         <f>B38+B39</f>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="4">
+        <v>53</v>
+      </c>
+      <c r="B41" s="14">
         <f>B40*0.19</f>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="10">
+        <v>54</v>
+      </c>
+      <c r="B42" s="15">
         <f>MAX(0,B37-B41)</f>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="10">
+        <v>55</v>
+      </c>
+      <c r="B43" s="15">
         <f>B42</f>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="4">
+        <v>23</v>
+      </c>
+      <c r="B47" s="14">
         <f>B43</f>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="4">
+        <v>24</v>
+      </c>
+      <c r="B48" s="14">
         <f>B47/12</f>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="10">
+        <v>26</v>
+      </c>
+      <c r="B49" s="15">
         <f>B10-B15-B47</f>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="10">
+        <v>27</v>
+      </c>
+      <c r="B50" s="15">
         <f>B49/12</f>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="10">
+        <v>28</v>
+      </c>
+      <c r="B51" s="15">
         <f>B49-(PRIVATE_COSTS*12)</f>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="10">
+        <v>29</v>
+      </c>
+      <c r="B52" s="15">
         <f>B51/12</f>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="6">
+        <v>25</v>
+      </c>
+      <c r="B53" s="21">
         <f>IFERROR(B47/B16,0)</f>
       </c>
     </row>
@@ -1579,38 +1722,38 @@
     <mergeCell ref="A45:C45"/>
   </mergeCells>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="between">
       <formula>0.3</formula>
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="lessThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1636,405 +1779,405 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="9">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13">
         <v>6000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="9">
+        <v>17</v>
+      </c>
+      <c r="B4" s="13">
         <v>1500</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="9">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9">
+        <v>31</v>
+      </c>
+      <c r="B6" s="13">
         <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14">
         <f>B3*12</f>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4">
+        <v>33</v>
+      </c>
+      <c r="B11" s="14">
         <f>B4*12</f>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="4">
+        <v>34</v>
+      </c>
+      <c r="B12" s="14">
         <f>B5*12</f>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4">
+        <v>35</v>
+      </c>
+      <c r="B13" s="14">
         <f>B6*12</f>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4">
+        <v>36</v>
+      </c>
+      <c r="B14" s="14">
         <f>RETA_ANNUAL</f>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="10">
+        <v>21</v>
+      </c>
+      <c r="B15" s="15">
         <f>SUM(B11:B14)</f>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="10">
+        <v>37</v>
+      </c>
+      <c r="B16" s="15">
         <f>B10-B15</f>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="4">
+        <v>37</v>
+      </c>
+      <c r="B20" s="14">
         <f>B16</f>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="4">
+        <v>39</v>
+      </c>
+      <c r="B21" s="14">
         <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15">
         <f>MAX(0,B16-B21)</f>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>40</v>
+      <c r="A25" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="17">
         <v>0</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="17">
         <v>12450</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="18">
         <v>0.19</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="14">
         <f>MAX(0,MIN($B$22,12450)-0)</f>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="14">
         <f>D26*C26</f>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="17">
         <v>12450</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="17">
         <v>20200</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="18">
         <v>0.24</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="14">
         <f>MAX(0,MIN($B$22,20200)-12450)</f>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="14">
         <f>D27*C27</f>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="17">
         <v>20200</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="17">
         <v>35200</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="18">
         <v>0.3</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="14">
         <f>MAX(0,MIN($B$22,35200)-20200)</f>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="14">
         <f>D28*C28</f>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="17">
         <v>35200</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="17">
         <v>60000</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="18">
         <v>0.37</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="14">
         <f>MAX(0,MIN($B$22,60000)-35200)</f>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="14">
         <f>D29*C29</f>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="17">
         <v>60000</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="17">
         <v>300000</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="18">
         <v>0.45</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="14">
         <f>MAX(0,MIN($B$22,300000)-60000)</f>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="14">
         <f>D30*C30</f>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="17">
         <v>300000</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="8">
+        <v>46</v>
+      </c>
+      <c r="C31" s="18">
         <v>0.47</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="14">
         <f>MAX(0,MIN($B$22,999999999)-300000)</f>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="14">
         <f>D31*C31</f>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="10">
+      <c r="A32" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="15">
         <f>SUM(E26:E31)</f>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="4">
+        <v>22</v>
+      </c>
+      <c r="B36" s="14">
         <f>B22</f>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="4">
+        <v>49</v>
+      </c>
+      <c r="B37" s="14">
         <f>E32</f>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="5">
+        <v>50</v>
+      </c>
+      <c r="B38" s="17">
         <f>MINIMO_PERSONAL</f>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="5">
+        <v>51</v>
+      </c>
+      <c r="B39" s="17">
         <f>MINIMO_DESCENDIENTES</f>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="11">
+        <v>52</v>
+      </c>
+      <c r="B40" s="20">
         <f>B38+B39</f>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="4">
+        <v>53</v>
+      </c>
+      <c r="B41" s="14">
         <f>B40*0.19</f>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="10">
+        <v>54</v>
+      </c>
+      <c r="B42" s="15">
         <f>MAX(0,B37-B41)</f>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="10">
+        <v>55</v>
+      </c>
+      <c r="B43" s="15">
         <f>B42</f>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="4">
+        <v>23</v>
+      </c>
+      <c r="B47" s="14">
         <f>B43</f>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="4">
+        <v>24</v>
+      </c>
+      <c r="B48" s="14">
         <f>B47/12</f>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="10">
+        <v>26</v>
+      </c>
+      <c r="B49" s="15">
         <f>B10-B15-B47</f>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="10">
+        <v>27</v>
+      </c>
+      <c r="B50" s="15">
         <f>B49/12</f>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="10">
+        <v>28</v>
+      </c>
+      <c r="B51" s="15">
         <f>B49-(PRIVATE_COSTS*12)</f>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="10">
+        <v>29</v>
+      </c>
+      <c r="B52" s="15">
         <f>B51/12</f>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="6">
+        <v>25</v>
+      </c>
+      <c r="B53" s="21">
         <f>IFERROR(B47/B16,0)</f>
       </c>
     </row>
@@ -2048,38 +2191,38 @@
     <mergeCell ref="A45:C45"/>
   </mergeCells>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="between">
       <formula>0.3</formula>
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="lessThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2105,405 +2248,405 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="9">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13">
         <v>9000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="9">
+        <v>17</v>
+      </c>
+      <c r="B4" s="13">
         <v>3000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="9">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13">
         <v>2500</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9">
+        <v>31</v>
+      </c>
+      <c r="B6" s="13">
         <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14">
         <f>B3*12</f>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4">
+        <v>33</v>
+      </c>
+      <c r="B11" s="14">
         <f>B4*12</f>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="4">
+        <v>34</v>
+      </c>
+      <c r="B12" s="14">
         <f>B5*12</f>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4">
+        <v>35</v>
+      </c>
+      <c r="B13" s="14">
         <f>B6*12</f>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4">
+        <v>36</v>
+      </c>
+      <c r="B14" s="14">
         <f>RETA_ANNUAL</f>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="10">
+        <v>21</v>
+      </c>
+      <c r="B15" s="15">
         <f>SUM(B11:B14)</f>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="10">
+        <v>37</v>
+      </c>
+      <c r="B16" s="15">
         <f>B10-B15</f>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="4">
+        <v>37</v>
+      </c>
+      <c r="B20" s="14">
         <f>B16</f>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="4">
+        <v>39</v>
+      </c>
+      <c r="B21" s="14">
         <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15">
         <f>MAX(0,B16-B21)</f>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>40</v>
+      <c r="A25" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="17">
         <v>0</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="17">
         <v>12450</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="18">
         <v>0.19</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="14">
         <f>MAX(0,MIN($B$22,12450)-0)</f>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="14">
         <f>D26*C26</f>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="17">
         <v>12450</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="17">
         <v>20200</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="18">
         <v>0.24</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="14">
         <f>MAX(0,MIN($B$22,20200)-12450)</f>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="14">
         <f>D27*C27</f>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="17">
         <v>20200</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="17">
         <v>35200</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="18">
         <v>0.3</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="14">
         <f>MAX(0,MIN($B$22,35200)-20200)</f>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="14">
         <f>D28*C28</f>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="17">
         <v>35200</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="17">
         <v>60000</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="18">
         <v>0.37</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="14">
         <f>MAX(0,MIN($B$22,60000)-35200)</f>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="14">
         <f>D29*C29</f>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="17">
         <v>60000</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="17">
         <v>300000</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="18">
         <v>0.45</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="14">
         <f>MAX(0,MIN($B$22,300000)-60000)</f>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="14">
         <f>D30*C30</f>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="17">
         <v>300000</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="8">
+        <v>46</v>
+      </c>
+      <c r="C31" s="18">
         <v>0.47</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="14">
         <f>MAX(0,MIN($B$22,999999999)-300000)</f>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="14">
         <f>D31*C31</f>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="10">
+      <c r="A32" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="15">
         <f>SUM(E26:E31)</f>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="4">
+        <v>22</v>
+      </c>
+      <c r="B36" s="14">
         <f>B22</f>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="4">
+        <v>49</v>
+      </c>
+      <c r="B37" s="14">
         <f>E32</f>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="5">
+        <v>50</v>
+      </c>
+      <c r="B38" s="17">
         <f>MINIMO_PERSONAL</f>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="5">
+        <v>51</v>
+      </c>
+      <c r="B39" s="17">
         <f>MINIMO_DESCENDIENTES</f>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="11">
+        <v>52</v>
+      </c>
+      <c r="B40" s="20">
         <f>B38+B39</f>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="4">
+        <v>53</v>
+      </c>
+      <c r="B41" s="14">
         <f>B40*0.19</f>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="10">
+        <v>54</v>
+      </c>
+      <c r="B42" s="15">
         <f>MAX(0,B37-B41)</f>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="10">
+        <v>55</v>
+      </c>
+      <c r="B43" s="15">
         <f>B42</f>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="4">
+        <v>23</v>
+      </c>
+      <c r="B47" s="14">
         <f>B43</f>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="4">
+        <v>24</v>
+      </c>
+      <c r="B48" s="14">
         <f>B47/12</f>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="10">
+        <v>26</v>
+      </c>
+      <c r="B49" s="15">
         <f>B10-B15-B47</f>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="10">
+        <v>27</v>
+      </c>
+      <c r="B50" s="15">
         <f>B49/12</f>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="10">
+        <v>28</v>
+      </c>
+      <c r="B51" s="15">
         <f>B49-(PRIVATE_COSTS*12)</f>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="10">
+        <v>29</v>
+      </c>
+      <c r="B52" s="15">
         <f>B51/12</f>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="6">
+        <v>25</v>
+      </c>
+      <c r="B53" s="21">
         <f>IFERROR(B47/B16,0)</f>
       </c>
     </row>
@@ -2517,38 +2660,38 @@
     <mergeCell ref="A45:C45"/>
   </mergeCells>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="between">
       <formula>0.3</formula>
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="9" operator="lessThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2574,405 +2717,405 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="9">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13">
         <v>12000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="9">
+        <v>17</v>
+      </c>
+      <c r="B4" s="13">
         <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="9">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13">
         <v>2500</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9">
+        <v>31</v>
+      </c>
+      <c r="B6" s="13">
         <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14">
         <f>B3*12</f>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4">
+        <v>33</v>
+      </c>
+      <c r="B11" s="14">
         <f>B4*12</f>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="4">
+        <v>34</v>
+      </c>
+      <c r="B12" s="14">
         <f>B5*12</f>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4">
+        <v>35</v>
+      </c>
+      <c r="B13" s="14">
         <f>B6*12</f>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4">
+        <v>36</v>
+      </c>
+      <c r="B14" s="14">
         <f>RETA_ANNUAL</f>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="10">
+        <v>21</v>
+      </c>
+      <c r="B15" s="15">
         <f>SUM(B11:B14)</f>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="10">
+        <v>37</v>
+      </c>
+      <c r="B16" s="15">
         <f>B10-B15</f>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="4">
+        <v>37</v>
+      </c>
+      <c r="B20" s="14">
         <f>B16</f>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="4">
+        <v>39</v>
+      </c>
+      <c r="B21" s="14">
         <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15">
         <f>MAX(0,B16-B21)</f>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>40</v>
+      <c r="A25" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="17">
         <v>0</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="17">
         <v>12450</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="18">
         <v>0.19</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="14">
         <f>MAX(0,MIN($B$22,12450)-0)</f>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="14">
         <f>D26*C26</f>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="17">
         <v>12450</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="17">
         <v>20200</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="18">
         <v>0.24</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="14">
         <f>MAX(0,MIN($B$22,20200)-12450)</f>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="14">
         <f>D27*C27</f>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="17">
         <v>20200</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="17">
         <v>35200</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="18">
         <v>0.3</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="14">
         <f>MAX(0,MIN($B$22,35200)-20200)</f>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="14">
         <f>D28*C28</f>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="17">
         <v>35200</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="17">
         <v>60000</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="18">
         <v>0.37</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="14">
         <f>MAX(0,MIN($B$22,60000)-35200)</f>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="14">
         <f>D29*C29</f>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="17">
         <v>60000</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="17">
         <v>300000</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="18">
         <v>0.45</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="14">
         <f>MAX(0,MIN($B$22,300000)-60000)</f>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="14">
         <f>D30*C30</f>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="17">
         <v>300000</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="8">
+        <v>46</v>
+      </c>
+      <c r="C31" s="18">
         <v>0.47</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="14">
         <f>MAX(0,MIN($B$22,999999999)-300000)</f>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="14">
         <f>D31*C31</f>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="10">
+      <c r="A32" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="15">
         <f>SUM(E26:E31)</f>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="4">
+        <v>22</v>
+      </c>
+      <c r="B36" s="14">
         <f>B22</f>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="4">
+        <v>49</v>
+      </c>
+      <c r="B37" s="14">
         <f>E32</f>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="5">
+        <v>50</v>
+      </c>
+      <c r="B38" s="17">
         <f>MINIMO_PERSONAL</f>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="5">
+        <v>51</v>
+      </c>
+      <c r="B39" s="17">
         <f>MINIMO_DESCENDIENTES</f>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="11">
+        <v>52</v>
+      </c>
+      <c r="B40" s="20">
         <f>B38+B39</f>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="4">
+        <v>53</v>
+      </c>
+      <c r="B41" s="14">
         <f>B40*0.19</f>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="10">
+        <v>54</v>
+      </c>
+      <c r="B42" s="15">
         <f>MAX(0,B37-B41)</f>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="10">
+        <v>55</v>
+      </c>
+      <c r="B43" s="15">
         <f>B42</f>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="4">
+        <v>23</v>
+      </c>
+      <c r="B47" s="14">
         <f>B43</f>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="4">
+        <v>24</v>
+      </c>
+      <c r="B48" s="14">
         <f>B47/12</f>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="10">
+        <v>26</v>
+      </c>
+      <c r="B49" s="15">
         <f>B10-B15-B47</f>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="10">
+        <v>27</v>
+      </c>
+      <c r="B50" s="15">
         <f>B49/12</f>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="10">
+        <v>28</v>
+      </c>
+      <c r="B51" s="15">
         <f>B49-(PRIVATE_COSTS*12)</f>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="10">
+        <v>29</v>
+      </c>
+      <c r="B52" s="15">
         <f>B51/12</f>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="6">
+        <v>25</v>
+      </c>
+      <c r="B53" s="21">
         <f>IFERROR(B47/B16,0)</f>
       </c>
     </row>
@@ -2986,38 +3129,38 @@
     <mergeCell ref="A45:C45"/>
   </mergeCells>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="6" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="7" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="8" operator="between">
       <formula>0.3</formula>
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="9" operator="lessThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3043,405 +3186,405 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="9">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13">
         <v>18000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="9">
+        <v>17</v>
+      </c>
+      <c r="B4" s="13">
         <v>8000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="9">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13">
         <v>2500</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9">
+        <v>31</v>
+      </c>
+      <c r="B6" s="13">
         <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14">
         <f>B3*12</f>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4">
+        <v>33</v>
+      </c>
+      <c r="B11" s="14">
         <f>B4*12</f>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="4">
+        <v>34</v>
+      </c>
+      <c r="B12" s="14">
         <f>B5*12</f>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4">
+        <v>35</v>
+      </c>
+      <c r="B13" s="14">
         <f>B6*12</f>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4">
+        <v>36</v>
+      </c>
+      <c r="B14" s="14">
         <f>RETA_ANNUAL</f>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="10">
+        <v>21</v>
+      </c>
+      <c r="B15" s="15">
         <f>SUM(B11:B14)</f>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="10">
+        <v>37</v>
+      </c>
+      <c r="B16" s="15">
         <f>B10-B15</f>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="4">
+        <v>37</v>
+      </c>
+      <c r="B20" s="14">
         <f>B16</f>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="4">
+        <v>39</v>
+      </c>
+      <c r="B21" s="14">
         <f>MIN(MAX(0,B16)*GASTOS_DIFICIL_RATE,GASTOS_DIFICIL_MAX)</f>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15">
         <f>MAX(0,B16-B21)</f>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>40</v>
+      <c r="A25" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="17">
         <v>0</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="17">
         <v>12450</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="18">
         <v>0.19</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="14">
         <f>MAX(0,MIN($B$22,12450)-0)</f>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="14">
         <f>D26*C26</f>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="17">
         <v>12450</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="17">
         <v>20200</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="18">
         <v>0.24</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="14">
         <f>MAX(0,MIN($B$22,20200)-12450)</f>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="14">
         <f>D27*C27</f>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="17">
         <v>20200</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="17">
         <v>35200</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="18">
         <v>0.3</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="14">
         <f>MAX(0,MIN($B$22,35200)-20200)</f>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="14">
         <f>D28*C28</f>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="17">
         <v>35200</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="17">
         <v>60000</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="18">
         <v>0.37</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="14">
         <f>MAX(0,MIN($B$22,60000)-35200)</f>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="14">
         <f>D29*C29</f>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="17">
         <v>60000</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="17">
         <v>300000</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="18">
         <v>0.45</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="14">
         <f>MAX(0,MIN($B$22,300000)-60000)</f>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="14">
         <f>D30*C30</f>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="17">
         <v>300000</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="8">
+        <v>46</v>
+      </c>
+      <c r="C31" s="18">
         <v>0.47</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="14">
         <f>MAX(0,MIN($B$22,999999999)-300000)</f>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="14">
         <f>D31*C31</f>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="10">
+      <c r="A32" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="15">
         <f>SUM(E26:E31)</f>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="4">
+        <v>22</v>
+      </c>
+      <c r="B36" s="14">
         <f>B22</f>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="4">
+        <v>49</v>
+      </c>
+      <c r="B37" s="14">
         <f>E32</f>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="5">
+        <v>50</v>
+      </c>
+      <c r="B38" s="17">
         <f>MINIMO_PERSONAL</f>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="5">
+        <v>51</v>
+      </c>
+      <c r="B39" s="17">
         <f>MINIMO_DESCENDIENTES</f>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="11">
+        <v>52</v>
+      </c>
+      <c r="B40" s="20">
         <f>B38+B39</f>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="4">
+        <v>53</v>
+      </c>
+      <c r="B41" s="14">
         <f>B40*0.19</f>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="10">
+        <v>54</v>
+      </c>
+      <c r="B42" s="15">
         <f>MAX(0,B37-B41)</f>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="10">
+        <v>55</v>
+      </c>
+      <c r="B43" s="15">
         <f>B42</f>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="4">
+        <v>23</v>
+      </c>
+      <c r="B47" s="14">
         <f>B43</f>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="4">
+        <v>24</v>
+      </c>
+      <c r="B48" s="14">
         <f>B47/12</f>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="10">
+        <v>26</v>
+      </c>
+      <c r="B49" s="15">
         <f>B10-B15-B47</f>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="10">
+        <v>27</v>
+      </c>
+      <c r="B50" s="15">
         <f>B49/12</f>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="10">
+        <v>28</v>
+      </c>
+      <c r="B51" s="15">
         <f>B49-(PRIVATE_COSTS*12)</f>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="10">
+        <v>29</v>
+      </c>
+      <c r="B52" s="15">
         <f>B51/12</f>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="6">
+        <v>25</v>
+      </c>
+      <c r="B53" s="21">
         <f>IFERROR(B47/B16,0)</f>
       </c>
     </row>
@@ -3455,38 +3598,38 @@
     <mergeCell ref="A45:C45"/>
   </mergeCells>
   <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="3" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="5" operator="between">
       <formula>0</formula>
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="6" operator="greaterThanOrEqual">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="7" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="49" priority="8" operator="between">
       <formula>0.3</formula>
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="9" operator="lessThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3498,4 +3641,422 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="13" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="8">
+        <f>'Scenario A - 3K'!B3</f>
+      </c>
+      <c r="C14" s="8">
+        <f>'Scenario B - 6K'!B3</f>
+      </c>
+      <c r="D14" s="8">
+        <f>'Scenario C - 9K'!B3</f>
+      </c>
+      <c r="E14" s="8">
+        <f>'Scenario D - 12K'!B3</f>
+      </c>
+      <c r="F14" s="8">
+        <f>'Scenario E - 18K'!B3</f>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="10">
+        <f>'Scenario A - 3K'!B4</f>
+      </c>
+      <c r="C15" s="10">
+        <f>'Scenario B - 6K'!B4</f>
+      </c>
+      <c r="D15" s="10">
+        <f>'Scenario C - 9K'!B4</f>
+      </c>
+      <c r="E15" s="10">
+        <f>'Scenario D - 12K'!B4</f>
+      </c>
+      <c r="F15" s="10">
+        <f>'Scenario E - 18K'!B4</f>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="11">
+        <f>'Scenario A - 3K'!B5</f>
+      </c>
+      <c r="C16" s="11">
+        <f>'Scenario B - 6K'!B5</f>
+      </c>
+      <c r="D16" s="11">
+        <f>'Scenario C - 9K'!B5</f>
+      </c>
+      <c r="E16" s="11">
+        <f>'Scenario D - 12K'!B5</f>
+      </c>
+      <c r="F16" s="11">
+        <f>'Scenario E - 18K'!B5</f>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="8">
+        <f>'Scenario A - 3K'!B10</f>
+      </c>
+      <c r="C18" s="8">
+        <f>'Scenario B - 6K'!B10</f>
+      </c>
+      <c r="D18" s="8">
+        <f>'Scenario C - 9K'!B10</f>
+      </c>
+      <c r="E18" s="8">
+        <f>'Scenario D - 12K'!B10</f>
+      </c>
+      <c r="F18" s="8">
+        <f>'Scenario E - 18K'!B10</f>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="10">
+        <f>'Scenario A - 3K'!B15</f>
+      </c>
+      <c r="C19" s="10">
+        <f>'Scenario B - 6K'!B15</f>
+      </c>
+      <c r="D19" s="10">
+        <f>'Scenario C - 9K'!B15</f>
+      </c>
+      <c r="E19" s="10">
+        <f>'Scenario D - 12K'!B15</f>
+      </c>
+      <c r="F19" s="10">
+        <f>'Scenario E - 18K'!B15</f>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="8">
+        <f>'Scenario A - 3K'!B22</f>
+      </c>
+      <c r="C20" s="8">
+        <f>'Scenario B - 6K'!B22</f>
+      </c>
+      <c r="D20" s="8">
+        <f>'Scenario C - 9K'!B22</f>
+      </c>
+      <c r="E20" s="8">
+        <f>'Scenario D - 12K'!B22</f>
+      </c>
+      <c r="F20" s="8">
+        <f>'Scenario E - 18K'!B22</f>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="8">
+        <f>'Scenario A - 3K'!B47</f>
+      </c>
+      <c r="C22" s="8">
+        <f>'Scenario B - 6K'!B47</f>
+      </c>
+      <c r="D22" s="8">
+        <f>'Scenario C - 9K'!B47</f>
+      </c>
+      <c r="E22" s="8">
+        <f>'Scenario D - 12K'!B47</f>
+      </c>
+      <c r="F22" s="8">
+        <f>'Scenario E - 18K'!B47</f>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="10">
+        <f>'Scenario A - 3K'!B48</f>
+      </c>
+      <c r="C23" s="10">
+        <f>'Scenario B - 6K'!B48</f>
+      </c>
+      <c r="D23" s="10">
+        <f>'Scenario C - 9K'!B48</f>
+      </c>
+      <c r="E23" s="10">
+        <f>'Scenario D - 12K'!B48</f>
+      </c>
+      <c r="F23" s="10">
+        <f>'Scenario E - 18K'!B48</f>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="12">
+        <f>'Scenario A - 3K'!B53</f>
+      </c>
+      <c r="C24" s="12">
+        <f>'Scenario B - 6K'!B53</f>
+      </c>
+      <c r="D24" s="12">
+        <f>'Scenario C - 9K'!B53</f>
+      </c>
+      <c r="E24" s="12">
+        <f>'Scenario D - 12K'!B53</f>
+      </c>
+      <c r="F24" s="12">
+        <f>'Scenario E - 18K'!B53</f>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="8">
+        <f>'Scenario A - 3K'!B49</f>
+      </c>
+      <c r="C26" s="8">
+        <f>'Scenario B - 6K'!B49</f>
+      </c>
+      <c r="D26" s="8">
+        <f>'Scenario C - 9K'!B49</f>
+      </c>
+      <c r="E26" s="8">
+        <f>'Scenario D - 12K'!B49</f>
+      </c>
+      <c r="F26" s="8">
+        <f>'Scenario E - 18K'!B49</f>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="10">
+        <f>'Scenario A - 3K'!B50</f>
+      </c>
+      <c r="C27" s="10">
+        <f>'Scenario B - 6K'!B50</f>
+      </c>
+      <c r="D27" s="10">
+        <f>'Scenario C - 9K'!B50</f>
+      </c>
+      <c r="E27" s="10">
+        <f>'Scenario D - 12K'!B50</f>
+      </c>
+      <c r="F27" s="10">
+        <f>'Scenario E - 18K'!B50</f>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="8">
+        <f>'Scenario A - 3K'!B51</f>
+      </c>
+      <c r="C28" s="8">
+        <f>'Scenario B - 6K'!B51</f>
+      </c>
+      <c r="D28" s="8">
+        <f>'Scenario C - 9K'!B51</f>
+      </c>
+      <c r="E28" s="8">
+        <f>'Scenario D - 12K'!B51</f>
+      </c>
+      <c r="F28" s="8">
+        <f>'Scenario E - 18K'!B51</f>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="10">
+        <f>'Scenario A - 3K'!B52</f>
+      </c>
+      <c r="C29" s="10">
+        <f>'Scenario B - 6K'!B52</f>
+      </c>
+      <c r="D29" s="10">
+        <f>'Scenario C - 9K'!B52</f>
+      </c>
+      <c r="E29" s="10">
+        <f>'Scenario D - 12K'!B52</f>
+      </c>
+      <c r="F29" s="10">
+        <f>'Scenario E - 18K'!B52</f>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A12:F12"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B28:F28">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:F29">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+      <formula>0</formula>
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" location="#'Scenario A - 3K'!A1"/>
+    <hyperlink ref="A6" r:id="rId2" location="#'Scenario B - 6K'!A1"/>
+    <hyperlink ref="A7" r:id="rId3" location="#'Scenario C - 9K'!A1"/>
+    <hyperlink ref="A8" r:id="rId4" location="#'Scenario D - 12K'!A1"/>
+    <hyperlink ref="A9" r:id="rId5" location="#'Scenario E - 18K'!A1"/>
+    <hyperlink ref="A10" r:id="rId6" location="#'Constants'!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(06-03): add print layout and sheet protection
- Print layout for Overview: landscape, fit to 1 page, header/footer
- Print layout for Scenario sheets: portrait, fit to width
- Print layout for Constants: portrait, header "Fiscal Constants 2025/2026"
- Sheet protection on Constants (prevents accidental edits)
- Generator note added as cell comment in Overview A1
- All sheets have margins and print areas configured

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/autonomo_calculator.xlsx
+++ b/autonomo_calculator.xlsx
@@ -20,9 +20,43 @@
     <definedName name="GASTOS_DIFICIL_RATE">Constants!$B$13</definedName>
     <definedName name="GASTOS_DIFICIL_MAX">Constants!$B$14</definedName>
     <definedName name="PRIVATE_COSTS">Constants!$B$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Overview'!$A1:$F30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Scenario A - 3K'!$A1:$E55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Scenario B - 6K'!$A1:$E55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Scenario C - 9K'!$A1:$E55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Scenario D - 12K'!$A1:$E55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Scenario E - 18K'!$A1:$E55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Constants'!$A1:$D31</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+          </rPr>
+          <t xml:space="preserve">Generated by autonomo_calculator
+</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+          </rPr>
+          <t>Node.js + ExcelJS</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1068,6 +1102,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -1290,16 +1327,24 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Fiscal Constants 2025/2026</oddHeader>
+    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -1762,13 +1807,20 @@
       <formula1>"1000,2500"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario A - 3K | Spanish Autonomo Tax Calculator</oddHeader>
+    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -2231,13 +2283,20 @@
       <formula1>"1000,2500"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario B - 6K | Spanish Autonomo Tax Calculator</oddHeader>
+    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -2700,13 +2759,20 @@
       <formula1>"1000,2500"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario C - 9K | Spanish Autonomo Tax Calculator</oddHeader>
+    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -3169,13 +3235,20 @@
       <formula1>"1000,2500"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario D - 12K | Spanish Autonomo Tax Calculator</oddHeader>
+    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -3638,13 +3711,20 @@
       <formula1>"1000,2500"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario E - 18K | Spanish Autonomo Tax Calculator</oddHeader>
+    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4056,7 +4136,12 @@
     <hyperlink ref="A9" r:id="rId5" location="#'Scenario E - 18K'!A1"/>
     <hyperlink ref="A10" r:id="rId6" location="#'Constants'!A1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" fitToWidth="1" fitToHeight="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Spanish Autonomo Tax Calculator - Overview</oddHeader>
+    <oddFooter>&amp;LPage &amp;P of &amp;N&amp;R&amp;D</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(06-03): translate Excel workbook to Dutch and remove Belgium dropdown
- Translate all labels, headers, and section titles to Dutch
- Remove Belgium Pattern dropdown validation (make it a regular editable input)
- All costs are now variable and flexible as per user request
- Sheet names changed: Overview -> Overzicht, Constants -> Constanten
- Generator console output also translated to Dutch

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/autonomo_calculator.xlsx
+++ b/autonomo_calculator.xlsx
@@ -4,29 +4,29 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="7" name="Overview" state="visible" r:id="rId4"/>
+    <sheet sheetId="7" name="Overzicht" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="Scenario A - 3K" state="visible" r:id="rId5"/>
     <sheet sheetId="3" name="Scenario B - 6K" state="visible" r:id="rId6"/>
     <sheet sheetId="4" name="Scenario C - 9K" state="visible" r:id="rId7"/>
     <sheet sheetId="5" name="Scenario D - 12K" state="visible" r:id="rId8"/>
     <sheet sheetId="6" name="Scenario E - 18K" state="visible" r:id="rId9"/>
-    <sheet sheetId="1" name="Constants" state="visible" r:id="rId10"/>
+    <sheet sheetId="1" name="Constanten" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="RETA_MONTHLY">Constants!$B$5</definedName>
-    <definedName name="RETA_ANNUAL">Constants!$B$6</definedName>
-    <definedName name="MINIMO_PERSONAL">Constants!$B$9</definedName>
-    <definedName name="MINIMO_DESCENDIENTES">Constants!$B$10</definedName>
-    <definedName name="GASTOS_DIFICIL_RATE">Constants!$B$13</definedName>
-    <definedName name="GASTOS_DIFICIL_MAX">Constants!$B$14</definedName>
-    <definedName name="PRIVATE_COSTS">Constants!$B$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Overview'!$A1:$F30</definedName>
+    <definedName name="RETA_MONTHLY">Constanten!$B$5</definedName>
+    <definedName name="RETA_ANNUAL">Constanten!$B$6</definedName>
+    <definedName name="MINIMO_PERSONAL">Constanten!$B$9</definedName>
+    <definedName name="MINIMO_DESCENDIENTES">Constanten!$B$10</definedName>
+    <definedName name="GASTOS_DIFICIL_RATE">Constanten!$B$13</definedName>
+    <definedName name="GASTOS_DIFICIL_MAX">Constanten!$B$14</definedName>
+    <definedName name="PRIVATE_COSTS">Constanten!$B$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Overzicht'!$A1:$F30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Scenario A - 3K'!$A1:$E55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Scenario B - 6K'!$A1:$E55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Scenario C - 9K'!$A1:$E55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Scenario D - 12K'!$A1:$E55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Scenario E - 18K'!$A1:$E55</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Constants'!$A1:$D31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Constanten'!$A1:$D31</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
@@ -44,7 +44,7 @@
           <rPr>
             <b/>
           </rPr>
-          <t xml:space="preserve">Generated by autonomo_calculator
+          <t xml:space="preserve">Gegenereerd door autonomo_calculator
 </t>
         </r>
         <r>
@@ -62,13 +62,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="74">
   <si>
-    <t>Spanish Autonomo Tax Calculator</t>
-  </si>
-  <si>
-    <t>Fiscal Year 2025/2026</t>
-  </si>
-  <si>
-    <t>Quick Navigation</t>
+    <t>Spaanse Autónomo Belasting Calculator</t>
+  </si>
+  <si>
+    <t>Fiscaal Jaar 2025/2026</t>
+  </si>
+  <si>
+    <t>Snelle Navigatie</t>
   </si>
   <si>
     <t>Scenario A - 3K</t>
@@ -86,13 +86,13 @@
     <t>Scenario E - 18K</t>
   </si>
   <si>
-    <t>Constants (Fiscal Data)</t>
-  </si>
-  <si>
-    <t>Scenario Comparison</t>
-  </si>
-  <si>
-    <t>Metric</t>
+    <t>Constanten (Fiscale Data)</t>
+  </si>
+  <si>
+    <t>Scenario Vergelijking</t>
+  </si>
+  <si>
+    <t>Metriek</t>
   </si>
   <si>
     <t>A</t>
@@ -110,178 +110,178 @@
     <t>E</t>
   </si>
   <si>
-    <t>Monthly Revenue</t>
-  </si>
-  <si>
-    <t>Monthly Expenses</t>
-  </si>
-  <si>
-    <t>Belgium Pattern</t>
+    <t>Maandelijkse Omzet</t>
+  </si>
+  <si>
+    <t>Maandelijkse Kosten</t>
+  </si>
+  <si>
+    <t>België Kosten</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Annual Revenue</t>
-  </si>
-  <si>
-    <t>Total Deductible</t>
+    <t>Jaarlijkse Omzet</t>
+  </si>
+  <si>
+    <t>Totaal Aftrekbaar</t>
   </si>
   <si>
     <t>Base Liquidable</t>
   </si>
   <si>
-    <t>Annual IRPF</t>
-  </si>
-  <si>
-    <t>Monthly IRPF</t>
-  </si>
-  <si>
-    <t>Effective Tax Rate</t>
-  </si>
-  <si>
-    <t>Annual Net Income</t>
-  </si>
-  <si>
-    <t>Monthly Net Income</t>
-  </si>
-  <si>
-    <t>Annual Leefgeld</t>
-  </si>
-  <si>
-    <t>Monthly Leefgeld</t>
-  </si>
-  <si>
-    <t>INPUTS (Edit these values)</t>
-  </si>
-  <si>
-    <t>Spain Deductible</t>
-  </si>
-  <si>
-    <t>ANNUAL CALCULATIONS</t>
-  </si>
-  <si>
-    <t>Annual Expenses</t>
-  </si>
-  <si>
-    <t>Annual Belgium Costs</t>
-  </si>
-  <si>
-    <t>Annual Spain Deductible</t>
-  </si>
-  <si>
-    <t>RETA Annual</t>
+    <t>Jaarlijkse IRPF</t>
+  </si>
+  <si>
+    <t>Maandelijkse IRPF</t>
+  </si>
+  <si>
+    <t>Effectief Belastingtarief</t>
+  </si>
+  <si>
+    <t>Jaarlijks Netto Inkomen</t>
+  </si>
+  <si>
+    <t>Maandelijks Netto Inkomen</t>
+  </si>
+  <si>
+    <t>Jaarlijks Leefgeld</t>
+  </si>
+  <si>
+    <t>Maandelijks Leefgeld</t>
+  </si>
+  <si>
+    <t>INVOER (Wijzig deze waarden)</t>
+  </si>
+  <si>
+    <t>Spanje Aftrekbaar</t>
+  </si>
+  <si>
+    <t>JAARLIJKSE BEREKENINGEN</t>
+  </si>
+  <si>
+    <t>Jaarlijkse Kosten</t>
+  </si>
+  <si>
+    <t>Jaarlijkse België Kosten</t>
+  </si>
+  <si>
+    <t>Jaarlijkse Spanje Aftrekbaar</t>
+  </si>
+  <si>
+    <t>RETA Jaarlijks</t>
   </si>
   <si>
     <t>Rendimiento Neto Previo</t>
   </si>
   <si>
-    <t>GASTOS DE DIFICIL JUSTIFICACION</t>
-  </si>
-  <si>
-    <t>Gastos Dificil (5%)</t>
-  </si>
-  <si>
-    <t>IRPF BRACKET CALCULATION</t>
-  </si>
-  <si>
-    <t>Lower</t>
-  </si>
-  <si>
-    <t>Upper</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Taxable</t>
-  </si>
-  <si>
-    <t>Tax</t>
+    <t>GASTOS DE DIFÍCIL JUSTIFICACIÓN</t>
+  </si>
+  <si>
+    <t>Gastos Difícil (5%)</t>
+  </si>
+  <si>
+    <t>IRPF SCHIJF BEREKENING</t>
+  </si>
+  <si>
+    <t>Ondergrens</t>
+  </si>
+  <si>
+    <t>Bovengrens</t>
+  </si>
+  <si>
+    <t>Tarief</t>
+  </si>
+  <si>
+    <t>Belastbaar</t>
+  </si>
+  <si>
+    <t>Belasting</t>
   </si>
   <si>
     <t>+</t>
   </si>
   <si>
-    <t>Total Tax (Cuota 1)</t>
-  </si>
-  <si>
-    <t>4-PHASE MINIMO METHOD</t>
-  </si>
-  <si>
-    <t>Tax on Base (Cuota 1)</t>
-  </si>
-  <si>
-    <t>Minimo Personal</t>
-  </si>
-  <si>
-    <t>Minimo Descendientes</t>
-  </si>
-  <si>
-    <t>Total Minimos</t>
-  </si>
-  <si>
-    <t>Tax on Minimos (Cuota 3)</t>
-  </si>
-  <si>
-    <t>Cuota Integra</t>
+    <t>Totale Belasting (Cuota 1)</t>
+  </si>
+  <si>
+    <t>4-FASE MÍNIMO METHODE</t>
+  </si>
+  <si>
+    <t>Belasting op Basis (Cuota 1)</t>
+  </si>
+  <si>
+    <t>Mínimo Personal</t>
+  </si>
+  <si>
+    <t>Mínimo Afstammelingen</t>
+  </si>
+  <si>
+    <t>Totaal Mínimos</t>
+  </si>
+  <si>
+    <t>Belasting op Mínimos (Cuota 3)</t>
+  </si>
+  <si>
+    <t>Cuota Íntegra</t>
   </si>
   <si>
     <t>Cuota Diferencial</t>
   </si>
   <si>
-    <t>FINAL RESULTS</t>
-  </si>
-  <si>
-    <t>Fiscal Data 2025/2026</t>
-  </si>
-  <si>
-    <t>Sources: AEAT, BOE, Seguridad Social</t>
-  </si>
-  <si>
-    <t>RETA (Seguridad Social)</t>
-  </si>
-  <si>
-    <t>RETA Monthly</t>
-  </si>
-  <si>
-    <t>Minimos Personales y Familiares</t>
-  </si>
-  <si>
-    <t>Minimo Descendientes (1)</t>
-  </si>
-  <si>
-    <t>Gastos de Dificil Justificacion</t>
-  </si>
-  <si>
-    <t>Gastos Dificil Rate</t>
-  </si>
-  <si>
-    <t>Gastos Dificil Max</t>
-  </si>
-  <si>
-    <t>Private Costs (Non-Deductible)</t>
-  </si>
-  <si>
-    <t>Private Costs Monthly</t>
-  </si>
-  <si>
-    <t>IRPF 2025 Brackets</t>
-  </si>
-  <si>
-    <t>Base Tax</t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>- RETA cuota is fixed from registration (not theoretical tramo)</t>
-  </si>
-  <si>
-    <t>- Gastos dificil: 5% (not 7% - that was exceptional 2023)</t>
-  </si>
-  <si>
-    <t>- Update these values for 2027 rates when available</t>
+    <t>EINDRESULTATEN</t>
+  </si>
+  <si>
+    <t>Fiscale Data 2025/2026</t>
+  </si>
+  <si>
+    <t>Bronnen: AEAT, BOE, Seguridad Social</t>
+  </si>
+  <si>
+    <t>RETA (Sociale Zekerheid)</t>
+  </si>
+  <si>
+    <t>RETA Maandelijks</t>
+  </si>
+  <si>
+    <t>Mínimos Personales y Familiares</t>
+  </si>
+  <si>
+    <t>Mínimo Afstammelingen (1)</t>
+  </si>
+  <si>
+    <t>Gastos de Difícil Justificación</t>
+  </si>
+  <si>
+    <t>Gastos Difícil Percentage</t>
+  </si>
+  <si>
+    <t>Gastos Difícil Maximum</t>
+  </si>
+  <si>
+    <t>Privé Kosten (Niet-Aftrekbaar)</t>
+  </si>
+  <si>
+    <t>Privé Kosten Maandelijks</t>
+  </si>
+  <si>
+    <t>IRPF 2025 Belastingschijven</t>
+  </si>
+  <si>
+    <t>Basis Belasting</t>
+  </si>
+  <si>
+    <t>Notities:</t>
+  </si>
+  <si>
+    <t>- RETA cuota is vast vanaf registratie (niet theoretische tramo)</t>
+  </si>
+  <si>
+    <t>- Gastos difícil: 5% (niet 7% - dat was uitzonderlijk in 2023)</t>
+  </si>
+  <si>
+    <t>- Werk deze waarden bij voor 2027 tarieven wanneer beschikbaar</t>
   </si>
 </sst>
 </file>
@@ -1334,8 +1334,8 @@
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Bold"Fiscal Constants 2025/2026</oddHeader>
-    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Fiscale Constanten 2025/2026</oddHeader>
+    <oddFooter>&amp;LPagina &amp;P&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1802,16 +1802,11 @@
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" sqref="B5">
-      <formula1>"1000,2500"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario A - 3K | Spanish Autonomo Tax Calculator</oddHeader>
-    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario A - 3K | Spaanse Autónomo Belasting Calculator</oddHeader>
+    <oddFooter>&amp;LPagina &amp;P&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2278,16 +2273,11 @@
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" sqref="B5">
-      <formula1>"1000,2500"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario B - 6K | Spanish Autonomo Tax Calculator</oddHeader>
-    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario B - 6K | Spaanse Autónomo Belasting Calculator</oddHeader>
+    <oddFooter>&amp;LPagina &amp;P&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2754,16 +2744,11 @@
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" sqref="B5">
-      <formula1>"1000,2500"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario C - 9K | Spanish Autonomo Tax Calculator</oddHeader>
-    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario C - 9K | Spaanse Autónomo Belasting Calculator</oddHeader>
+    <oddFooter>&amp;LPagina &amp;P&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3230,16 +3215,11 @@
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" sqref="B5">
-      <formula1>"1000,2500"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario D - 12K | Spanish Autonomo Tax Calculator</oddHeader>
-    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario D - 12K | Spaanse Autónomo Belasting Calculator</oddHeader>
+    <oddFooter>&amp;LPagina &amp;P&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3706,16 +3686,11 @@
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" sqref="B5">
-      <formula1>"1000,2500"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" fitToWidth="1" fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario E - 18K | Spanish Autonomo Tax Calculator</oddHeader>
-    <oddFooter>&amp;LPage &amp;P&amp;R&amp;D</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Scenario E - 18K | Spaanse Autónomo Belasting Calculator</oddHeader>
+    <oddFooter>&amp;LPagina &amp;P&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4134,13 +4109,13 @@
     <hyperlink ref="A7" r:id="rId3" location="#'Scenario C - 9K'!A1"/>
     <hyperlink ref="A8" r:id="rId4" location="#'Scenario D - 12K'!A1"/>
     <hyperlink ref="A9" r:id="rId5" location="#'Scenario E - 18K'!A1"/>
-    <hyperlink ref="A10" r:id="rId6" location="#'Constants'!A1"/>
+    <hyperlink ref="A10" r:id="rId6" location="#'Constanten'!A1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" fitToWidth="1" fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Bold"Spanish Autonomo Tax Calculator - Overview</oddHeader>
-    <oddFooter>&amp;LPage &amp;P of &amp;N&amp;R&amp;D</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Bold"Spaanse Autónomo Belasting Calculator - Overzicht</oddHeader>
+    <oddFooter>&amp;LPagina &amp;P van &amp;N&amp;R&amp;D</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId8"/>
 </worksheet>

</xml_diff>